<commit_message>
support images in xlsx
</commit_message>
<xml_diff>
--- a/core/test/smoketest/test.xlsx
+++ b/core/test/smoketest/test.xlsx
@@ -35,7 +35,7 @@
     <t>${col1} ${col2}</t>
   </si>
   <si>
-    <t>just split</t>
+    <t>${image}</t>
   </si>
 </sst>
 </file>
@@ -166,7 +166,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -495,10 +495,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -538,7 +541,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="108.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fix for multiple charts and multiple sheets
</commit_message>
<xml_diff>
--- a/core/test/smoketest/test.xlsx
+++ b/core/test/smoketest/test.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Band1">data!$A$1:$C$1</definedName>
     <definedName name="Band2">data!$D$1:$F$2</definedName>
     <definedName name="Band3">data!$A$3:$A$4</definedName>
-    <definedName name="Footer">data!$A$6:$I$22</definedName>
+    <definedName name="Footer">data!$A$6:$V$22</definedName>
+    <definedName name="Second">data2!$A$1:$K$18</definedName>
     <definedName name="Split">data!$A$5:$C$5</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>${col1}</t>
   </si>
@@ -37,12 +39,15 @@
   <si>
     <t>${image}</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,8 +56,32 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -62,6 +91,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -78,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -86,10 +121,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -108,6 +147,180 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
   <c:chart>
+    <c:title/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>График</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>${col1}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$B$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>График</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>${col1}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$B$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>${col1}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="64359424"/>
+        <c:axId val="64377600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="64359424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64377600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="64377600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64359424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
     <c:title>
       <c:layout/>
     </c:title>
@@ -115,6 +328,36 @@
       <c:layout/>
       <c:pieChart>
         <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>График</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>${col1}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$B$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -166,7 +409,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -176,20 +419,85 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -492,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -504,49 +812,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="108.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -557,6 +866,11 @@
       </c>
       <c r="C6" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="22:22">
+      <c r="V22" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -568,4 +882,254 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
allow to convert docx and xlsx to pdf through openoffice
</commit_message>
<xml_diff>
--- a/core/test/smoketest/test.xlsx
+++ b/core/test/smoketest/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -217,6 +219,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -232,7 +235,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -274,24 +277,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64359424"/>
-        <c:axId val="64377600"/>
+        <c:axId val="55905664"/>
+        <c:axId val="55923840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64359424"/>
+        <c:axId val="55905664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64377600"/>
+        <c:crossAx val="55923840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64377600"/>
+        <c:axId val="55923840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -299,19 +302,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64359424"/>
+        <c:crossAx val="55905664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -409,7 +413,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -419,16 +423,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -449,16 +453,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -802,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -888,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>

</xml_diff>